<commit_message>
Finishing appendix tables and figures
</commit_message>
<xml_diff>
--- a/results/figureA1_any_evidence.xlsx
+++ b/results/figureA1_any_evidence.xlsx
@@ -34,67 +34,67 @@
     <t>total_dof</t>
   </si>
   <si>
-    <t>(0.82)</t>
-  </si>
-  <si>
-    <t>(0.49)</t>
-  </si>
-  <si>
-    <t>(0.69)</t>
+    <t>(0.79)</t>
   </si>
   <si>
     <t>(0.5)</t>
   </si>
   <si>
-    <t>(0.88)</t>
+    <t>(0.7)</t>
+  </si>
+  <si>
+    <t>(0.46)</t>
+  </si>
+  <si>
+    <t>(0.92)</t>
+  </si>
+  <si>
+    <t>(0.59)</t>
+  </si>
+  <si>
+    <t>(0.89)</t>
+  </si>
+  <si>
+    <t>(0.68)</t>
+  </si>
+  <si>
+    <t>(0.96)</t>
+  </si>
+  <si>
+    <t>(0.64)</t>
+  </si>
+  <si>
+    <t>(0.9)</t>
+  </si>
+  <si>
+    <t>(1.04)</t>
+  </si>
+  <si>
+    <t>(0.8)</t>
+  </si>
+  <si>
+    <t>(0.94)</t>
+  </si>
+  <si>
+    <t>(0.73)</t>
+  </si>
+  <si>
+    <t>(0.95)</t>
+  </si>
+  <si>
+    <t>(0.67)</t>
+  </si>
+  <si>
+    <t>(0.65)</t>
   </si>
   <si>
     <t>(0.56)</t>
   </si>
   <si>
-    <t>(0.75)</t>
-  </si>
-  <si>
-    <t>(0.62)</t>
-  </si>
-  <si>
-    <t>(1.08)</t>
-  </si>
-  <si>
-    <t>(0.72)</t>
-  </si>
-  <si>
-    <t>(1.01)</t>
-  </si>
-  <si>
-    <t>(0.68)</t>
-  </si>
-  <si>
-    <t>(0.99)</t>
-  </si>
-  <si>
-    <t>(0.73)</t>
-  </si>
-  <si>
-    <t>(0.98)</t>
-  </si>
-  <si>
-    <t>(0.89)</t>
-  </si>
-  <si>
-    <t>(0.63)</t>
-  </si>
-  <si>
-    <t>(0.9)</t>
-  </si>
-  <si>
-    <t>(0.7)</t>
-  </si>
-  <si>
-    <t>(1.14)</t>
-  </si>
-  <si>
-    <t>(0.93)</t>
+    <t>(1.11)</t>
+  </si>
+  <si>
+    <t>(0.86)</t>
   </si>
 </sst>
 </file>
@@ -592,10 +592,10 @@
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
         <v>21</v>
@@ -665,13 +665,13 @@
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J6" t="s">
         <v>22</v>

</xml_diff>